<commit_message>
Tasks day 10  actions and cookies
</commit_message>
<xml_diff>
--- a/src/test/resources/excelfile.xlsx
+++ b/src/test/resources/excelfile.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\830-G7\Desktop\SelenuimJunit\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD08ED1-395C-4147-BBB9-80C45381F1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3106FEDE-F428-4B61-900B-9F7B12CA0146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12315" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
     <sheet name="Sayfa2" sheetId="2" r:id="rId2"/>
+    <sheet name="TestAutomation" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -77,12 +78,22 @@
   </si>
   <si>
     <t>Çin</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,8 +431,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
@@ -568,8 +579,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
@@ -679,4 +690,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>